<commit_message>
feat: Update CourseModal and validation schema to support optional QPNOS fields and improve form handling
</commit_message>
<xml_diff>
--- a/src/assets/Batch_Template-Instruction.xlsx
+++ b/src/assets/Batch_Template-Instruction.xlsx
@@ -1,27 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr codeName="ThisWorkbook"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TRITHANKA\Downloads\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3F590AF-24E1-454F-864C-AFCC3238E742}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView windowWidth="28800" windowHeight="12930" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="TemplateBatch Template" sheetId="1" r:id="rId1"/>
     <sheet name="InstructionSheet" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="40">
   <si>
     <t>Sl No</t>
   </si>
@@ -32,7 +26,10 @@
     <t>Course Name</t>
   </si>
   <si>
-    <t>SDMS ID</t>
+    <t>Trainner Name</t>
+  </si>
+  <si>
+    <t>Trainer PAN</t>
   </si>
   <si>
     <t>Start Date</t>
@@ -44,6 +41,12 @@
     <t>Batch Number</t>
   </si>
   <si>
+    <t>Target Order Number</t>
+  </si>
+  <si>
+    <t>Batch Target</t>
+  </si>
+  <si>
     <t>Field Name</t>
   </si>
   <si>
@@ -83,12 +86,6 @@
     <t>"Software Development"</t>
   </si>
   <si>
-    <t>NSDC batch Id</t>
-  </si>
-  <si>
-    <t>"SDMS12345"</t>
-  </si>
-  <si>
     <t>Date</t>
   </si>
   <si>
@@ -98,22 +95,47 @@
     <t>"2025-01-01"</t>
   </si>
   <si>
+    <t>"Trainner Name ABC"</t>
+  </si>
+  <si>
     <t>End date of the batch (must be later than Start Date, YYYY-MM-DD format)</t>
   </si>
   <si>
     <t>"2025-06-30"</t>
   </si>
   <si>
+    <t>Trainer PAN assigned to the Trainer</t>
+  </si>
+  <si>
+    <t>"PAN123G"</t>
+  </si>
+  <si>
     <t>Unique batch number</t>
   </si>
   <si>
     <t>101</t>
   </si>
   <si>
+    <t>Target Order Number associate with the Scheme</t>
+  </si>
+  <si>
+    <t>Tar123</t>
+  </si>
+  <si>
+    <t>Batch Size Enrolled</t>
+  </si>
+  <si>
     <t>INSTRUCTION</t>
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t xml:space="preserve">1. </t>
     </r>
     <r>
@@ -132,7 +154,7 @@
         <sz val="12"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <family val="2"/>
+        <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> If the heading names are changed, the system will show an error message.</t>
@@ -140,6 +162,88 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">2. To upload </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Batch details</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, make sure to </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>first upload Training Center (TC)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>,</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Trainer, Target and Course </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> details.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t xml:space="preserve">3. </t>
     </r>
     <r>
@@ -158,7 +262,7 @@
         <sz val="12"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <family val="2"/>
+        <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> should be </t>
@@ -179,7 +283,7 @@
         <sz val="12"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <family val="2"/>
+        <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> the </t>
@@ -196,109 +300,23 @@
       <t>Batch Start Date.</t>
     </r>
   </si>
-  <si>
-    <t>Batch Target</t>
-  </si>
-  <si>
-    <t>Target Order Number</t>
-  </si>
-  <si>
-    <t>Target Order Number associate with the Scheme</t>
-  </si>
-  <si>
-    <t>Tar123</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">2. To upload </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Batch details</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">, make sure to </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>first upload Training Center (TC)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>,</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Trainer, Target and Course </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> details.</t>
-    </r>
-  </si>
-  <si>
-    <t>Batch Size Enrolled</t>
-  </si>
-  <si>
-    <t>Trainer PAN</t>
-  </si>
-  <si>
-    <t>Trainer PAN assigned to the Trainer</t>
-  </si>
-  <si>
-    <t>"PAN123G"</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+  </numFmts>
+  <fonts count="23">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -317,16 +335,353 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -349,32 +704,318 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="58" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="60% - Accent6" xfId="1" builtinId="52"/>
+    <cellStyle name="40% - Accent6" xfId="2" builtinId="51"/>
+    <cellStyle name="60% - Accent5" xfId="3" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="4" builtinId="49"/>
+    <cellStyle name="40% - Accent5" xfId="5" builtinId="47"/>
+    <cellStyle name="20% - Accent5" xfId="6" builtinId="46"/>
+    <cellStyle name="60% - Accent4" xfId="7" builtinId="44"/>
+    <cellStyle name="Accent5" xfId="8" builtinId="45"/>
+    <cellStyle name="40% - Accent4" xfId="9" builtinId="43"/>
+    <cellStyle name="Accent4" xfId="10" builtinId="41"/>
+    <cellStyle name="Linked Cell" xfId="11" builtinId="24"/>
+    <cellStyle name="40% - Accent3" xfId="12" builtinId="39"/>
+    <cellStyle name="60% - Accent2" xfId="13" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="14" builtinId="37"/>
+    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
+    <cellStyle name="20% - Accent2" xfId="16" builtinId="34"/>
+    <cellStyle name="Accent2" xfId="17" builtinId="33"/>
+    <cellStyle name="40% - Accent1" xfId="18" builtinId="31"/>
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30"/>
+    <cellStyle name="Accent1" xfId="20" builtinId="29"/>
+    <cellStyle name="Neutral" xfId="21" builtinId="28"/>
+    <cellStyle name="60% - Accent1" xfId="22" builtinId="32"/>
+    <cellStyle name="Bad" xfId="23" builtinId="27"/>
+    <cellStyle name="20% - Accent4" xfId="24" builtinId="42"/>
+    <cellStyle name="Total" xfId="25" builtinId="25"/>
+    <cellStyle name="Output" xfId="26" builtinId="21"/>
+    <cellStyle name="Currency" xfId="27" builtinId="4"/>
+    <cellStyle name="20% - Accent3" xfId="28" builtinId="38"/>
+    <cellStyle name="Note" xfId="29" builtinId="10"/>
+    <cellStyle name="Input" xfId="30" builtinId="20"/>
+    <cellStyle name="Heading 4" xfId="31" builtinId="19"/>
+    <cellStyle name="Calculation" xfId="32" builtinId="22"/>
+    <cellStyle name="Good" xfId="33" builtinId="26"/>
+    <cellStyle name="Heading 3" xfId="34" builtinId="18"/>
+    <cellStyle name="CExplanatory Text" xfId="35" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="36" builtinId="16"/>
+    <cellStyle name="Comma [0]" xfId="37" builtinId="6"/>
+    <cellStyle name="20% - Accent6" xfId="38" builtinId="50"/>
+    <cellStyle name="Title" xfId="39" builtinId="15"/>
+    <cellStyle name="Currency [0]" xfId="40" builtinId="7"/>
+    <cellStyle name="Warning Text" xfId="41" builtinId="11"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9"/>
+    <cellStyle name="Heading 2" xfId="43" builtinId="17"/>
+    <cellStyle name="Comma" xfId="44" builtinId="3"/>
+    <cellStyle name="Check Cell" xfId="45" builtinId="23"/>
+    <cellStyle name="60% - Accent3" xfId="46" builtinId="40"/>
+    <cellStyle name="Percent" xfId="47" builtinId="5"/>
+    <cellStyle name="Hyperlink" xfId="48" builtinId="8"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -696,26 +1337,26 @@
       </a:style>
     </a:lnDef>
   </a:objectDefaults>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:J3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:J2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75" outlineLevelRow="2"/>
   <cols>
-    <col min="2" max="2" width="14.4140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.58203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="9.9140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.58203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.33203125" customWidth="1"/>
+    <col min="2" max="2" width="14.4133333333333" customWidth="1"/>
+    <col min="3" max="4" width="15.58" customWidth="1"/>
+    <col min="5" max="5" width="17.5" customWidth="1"/>
+    <col min="6" max="7" width="9.91333333333333" customWidth="1"/>
+    <col min="8" max="8" width="12.58" customWidth="1"/>
+    <col min="9" max="9" width="20.3333333333333" customWidth="1"/>
     <col min="10" max="10" width="13" customWidth="1"/>
   </cols>
   <sheetData>
@@ -730,79 +1371,81 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I1" t="s">
-        <v>33</v>
+        <v>8</v>
       </c>
       <c r="J1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10">
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-    </row>
-    <row r="3" spans="1:10">
-      <c r="D3" s="4"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="6:7">
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+    </row>
+    <row r="3" spans="5:7">
+      <c r="E3" s="4"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="date" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F1:G1048576" xr:uid="{973934A3-6696-41EB-B067-66B993C84317}">
+    <dataValidation type="date" operator="between" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F$1:G$1048576">
       <formula1>18264</formula1>
       <formula2>54789</formula2>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="1" orientation="portrait"/>
+  <headerFooter/>
   <ignoredErrors>
-    <ignoredError sqref="A1 B1:C1 E1" numberStoredAsText="1"/>
+    <ignoredError sqref="A1 B1:C1" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8117C17-74CA-4FE9-A9E3-75D65BB5F648}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="24.83203125" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="24.8333333333333" defaultRowHeight="15.75" outlineLevelCol="4"/>
   <cols>
-    <col min="4" max="4" width="61.08203125" customWidth="1"/>
+    <col min="4" max="4" width="61.08" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>11</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -810,16 +1453,16 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C2" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="D2" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E2" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -827,16 +1470,16 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="D3" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E3" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -844,156 +1487,157 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="D4" t="s">
         <v>2</v>
       </c>
       <c r="E4" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="D5" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="E5" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C6" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D6" t="s">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="E6" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C7" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D7" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="E7" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>38</v>
+        <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C8" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="D8" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="E8" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C9" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="D9" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="E9" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" t="s">
         <v>33</v>
       </c>
-      <c r="B10" t="s">
-        <v>8</v>
-      </c>
-      <c r="C10" t="s">
+      <c r="E10" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" t="s">
         <v>16</v>
       </c>
-      <c r="D10" t="s">
-        <v>34</v>
-      </c>
-      <c r="E10" t="s">
+      <c r="D11" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
-      <c r="A11" t="s">
-        <v>32</v>
-      </c>
-      <c r="B11" t="s">
-        <v>8</v>
-      </c>
-      <c r="C11" t="s">
-        <v>13</v>
-      </c>
-      <c r="D11" t="s">
+    <row r="13" spans="1:1">
+      <c r="A13" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" ht="26" customHeight="1" spans="1:1">
+      <c r="A14" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
-      <c r="A13" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="26" customHeight="1">
-      <c r="A14" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="26" customHeight="1">
+    <row r="15" ht="26" customHeight="1" spans="1:1">
       <c r="A15" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="26" customHeight="1">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="16" ht="26" customHeight="1" spans="1:1">
       <c r="A16" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>